<commit_message>
my april weekly report
</commit_message>
<xml_diff>
--- a/april_status/pawan_kakde_April.xlsx
+++ b/april_status/pawan_kakde_April.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="10Apr to 17Apr" sheetId="1" r:id="rId1"/>
-    <sheet name="18Apr to 24Apr" sheetId="2" r:id="rId2"/>
-    <sheet name="25Apr to1may" sheetId="4" r:id="rId3"/>
+    <sheet name="03Ape to 09Apr" sheetId="5" r:id="rId1"/>
+    <sheet name="10Apr to 17Apr" sheetId="1" r:id="rId2"/>
+    <sheet name="18Apr to 24Apr" sheetId="2" r:id="rId3"/>
+    <sheet name="25Apr to30Apr" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="99">
   <si>
     <t>HST.QUL;</t>
   </si>
@@ -159,9 +160,6 @@
     <t>2Hrs</t>
   </si>
   <si>
-    <t>2.5Hrs</t>
-  </si>
-  <si>
     <t>1.30Hrs</t>
   </si>
   <si>
@@ -213,9 +211,6 @@
     <t>1.45Hrs</t>
   </si>
   <si>
-    <t>2.25Hrs</t>
-  </si>
-  <si>
     <t>1.35Hrs</t>
   </si>
   <si>
@@ -226,13 +221,109 @@
   </si>
   <si>
     <t>April</t>
+  </si>
+  <si>
+    <t>monday</t>
+  </si>
+  <si>
+    <t>tuesday</t>
+  </si>
+  <si>
+    <t>wednesday</t>
+  </si>
+  <si>
+    <t>thursday</t>
+  </si>
+  <si>
+    <t>friday</t>
+  </si>
+  <si>
+    <t>saturday</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>Week number</t>
+  </si>
+  <si>
+    <t>About course (APSE)&amp;subjects</t>
+  </si>
+  <si>
+    <t>virtual box download&amp;installation</t>
+  </si>
+  <si>
+    <t>Linux &amp;Ubuntu(Terminal)</t>
+  </si>
+  <si>
+    <t>Download &amp;install Linux(ubuntu)</t>
+  </si>
+  <si>
+    <t>Ubuntu (Terminal open and try basic command)</t>
+  </si>
+  <si>
+    <t>Basic Excel practice</t>
+  </si>
+  <si>
+    <t>9.5Hrs</t>
+  </si>
+  <si>
+    <t>Github command (git init,git statut,git add,git commit,git push)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Github command untr…ed file modi..ed file.. Co..nd (git rm --cached *,git restore --staged) </t>
+  </si>
+  <si>
+    <t>How to create repostary</t>
+  </si>
+  <si>
+    <t>version control system</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>How to (APSE)course on waching youtube video</t>
+  </si>
+  <si>
+    <t>7Hrs</t>
+  </si>
+  <si>
+    <t>How to Excel on Waching youtube video</t>
+  </si>
+  <si>
+    <t>8Hrs</t>
+  </si>
+  <si>
+    <t>9.30Hrs</t>
+  </si>
+  <si>
+    <t>Basic microsoft excel</t>
+  </si>
+  <si>
+    <t>Linux command parctice</t>
+  </si>
+  <si>
+    <t>Email parctice</t>
+  </si>
+  <si>
+    <t>GIthub parctice</t>
+  </si>
+  <si>
+    <t>7.30Hrs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +400,83 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF0070C0"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF0070C0"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -318,7 +486,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -472,11 +640,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -505,9 +733,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -532,27 +757,119 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="7" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="15" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="15" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,268 +1179,258 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="63"/>
+      <c r="D2" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16" t="s">
+      <c r="E2" s="46"/>
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="17">
-        <v>44661</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" ht="36.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="E3" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="49"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="57">
+        <v>44654</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="49"/>
+    </row>
+    <row r="5" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="17">
-        <v>44668</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="18" t="s">
+      <c r="B5" s="57">
+        <v>44660</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="23" t="s">
+      <c r="F5" s="49"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16" t="s">
+      <c r="C6" s="39"/>
+      <c r="D6" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" s="7" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="20" t="s">
+      <c r="E6" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="49"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="49"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="48"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="49"/>
+    </row>
+    <row r="9" spans="1:6" s="70" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="66"/>
+      <c r="B9" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C9" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D9" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E9" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F9" s="69" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="24">
-        <v>44661</v>
-      </c>
-      <c r="C9" s="25" t="s">
+    <row r="10" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="83"/>
+      <c r="B10" s="61">
+        <v>44654</v>
+      </c>
+      <c r="C10" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="24">
-        <v>44662</v>
-      </c>
-      <c r="C10" s="25" t="s">
+      <c r="D10" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="84" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="83"/>
+      <c r="B11" s="61">
+        <v>44655</v>
+      </c>
+      <c r="C11" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="25" t="s">
+      <c r="D11" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="85"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="83"/>
+      <c r="B12" s="61">
+        <v>44656</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="85"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="83"/>
+      <c r="B13" s="61">
+        <v>44657</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="85" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="83"/>
+      <c r="B14" s="61">
+        <v>44658</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="85"/>
+    </row>
+    <row r="15" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="83"/>
+      <c r="B15" s="61">
+        <v>44659</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="24">
-        <v>44663</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="24">
-        <v>44664</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="24">
-        <v>44665</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="24">
-        <v>44666</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="25" t="s">
+      <c r="F15" s="84" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="86"/>
+      <c r="B16" s="65">
+        <v>44660</v>
+      </c>
+      <c r="C16" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="24">
-        <v>44667</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="29">
-        <v>44668</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="31"/>
+      <c r="E16" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="87"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1133,10 +1440,295 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="17">
+        <v>44661</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" ht="36.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="17">
+        <v>44668</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="36"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" s="7" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="23">
+        <v>44661</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="23">
+        <v>44662</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="23">
+        <v>44663</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="23">
+        <v>44664</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="23">
+        <v>44665</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="23">
+        <v>44666</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="23">
+        <v>44667</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="28">
+        <v>44668</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,245 +1744,245 @@
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="33"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="89"/>
     </row>
     <row r="3" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="37"/>
+      <c r="F3" s="85"/>
     </row>
     <row r="4" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="17">
         <v>44669</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="16"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="37"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="85"/>
     </row>
     <row r="5" spans="1:6" ht="36.75" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="17">
         <v>44675</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="85"/>
     </row>
     <row r="6" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="37"/>
+      <c r="E6" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="85"/>
     </row>
     <row r="7" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="37"/>
+      <c r="A7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="34">
+        <v>44652</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="85"/>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
+      <c r="A8" s="83"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="37"/>
-    </row>
-    <row r="9" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="42" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="85"/>
+    </row>
+    <row r="9" spans="1:6" s="78" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A9" s="90"/>
+      <c r="B9" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="91" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="24">
+      <c r="A10" s="83"/>
+      <c r="B10" s="23">
         <v>44669</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="26" t="s">
+      <c r="E10" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="92" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="83"/>
+      <c r="B11" s="23">
+        <v>44670</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="92" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="83"/>
+      <c r="B12" s="23">
+        <v>44671</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="92"/>
+    </row>
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="83"/>
+      <c r="B13" s="23">
+        <v>44672</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="93" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="24">
-        <v>44670</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="25" t="s">
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="83"/>
+      <c r="B14" s="23">
+        <v>44673</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E14" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="92"/>
+    </row>
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="83"/>
+      <c r="B15" s="23">
+        <v>44674</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="92" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="A16" s="83"/>
+      <c r="B16" s="23">
+        <v>44675</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="24">
-        <v>44671</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="26"/>
-    </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="24">
-        <v>44672</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="24">
-        <v>44673</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="26"/>
-    </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="24">
-        <v>44674</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="26" t="s">
+      <c r="F16" s="93" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="24">
-        <v>44675</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
     <row r="17" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="44"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
+      <c r="A17" s="86"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="87"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1398,14 +1990,262 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="94"/>
+      <c r="D2" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="46"/>
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="38">
+        <v>4</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="49"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="40">
+        <v>44676</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="49"/>
+    </row>
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="40">
+        <v>44681</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="49"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="80" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="49"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="49"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="48"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="49"/>
+    </row>
+    <row r="9" spans="1:6" s="75" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="72"/>
+      <c r="B9" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="74" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="50"/>
+      <c r="B10" s="79">
+        <v>44676</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="80" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="85" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="50"/>
+      <c r="B11" s="79">
+        <v>44677</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="85" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="50"/>
+      <c r="B12" s="79">
+        <v>44678</v>
+      </c>
+      <c r="C12" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="80" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="85"/>
+    </row>
+    <row r="13" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="50"/>
+      <c r="B13" s="79">
+        <v>44679</v>
+      </c>
+      <c r="C13" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="88" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="80" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="85" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="50"/>
+      <c r="B14" s="79">
+        <v>44680</v>
+      </c>
+      <c r="C14" s="80" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="88" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="85" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="50"/>
+      <c r="B15" s="79">
+        <v>44681</v>
+      </c>
+      <c r="C15" s="80" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="85" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="54"/>
+    </row>
+    <row r="17" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>